<commit_message>
Add logic filter testcase range
</commit_message>
<xml_diff>
--- a/Testcase_ZenS.xlsx
+++ b/Testcase_ZenS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Desktop/Test/automation-testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88CA6579-464D-6449-95DE-CC72C6ED88DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6695729-5008-1540-8B20-27D4CA5C67AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16100" activeTab="1" xr2:uid="{4693CEE1-BB04-3241-88A0-42DA0181BF78}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="59">
   <si>
     <t>TC ID</t>
   </si>
@@ -109,9 +109,6 @@
     <t>Login test (normal)</t>
   </si>
   <si>
-    <t>TC automation</t>
-  </si>
-  <si>
     <t>Action</t>
   </si>
   <si>
@@ -218,6 +215,15 @@
   </si>
   <si>
     <t>c</t>
+  </si>
+  <si>
+    <t>Login test (abnormal 3)</t>
+  </si>
+  <si>
+    <t>5. Check title after sign in (3)</t>
+  </si>
+  <si>
+    <t>abacasd</t>
   </si>
 </sst>
 </file>
@@ -799,20 +805,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5D6DBF1-623A-3743-A813-70ED5E468A4E}">
-  <dimension ref="A2:N39"/>
+  <dimension ref="A2:N41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="105" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="19.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="29.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" style="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="61.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="63.83203125" style="12" customWidth="1"/>
     <col min="8" max="8" width="37.1640625" style="18" customWidth="1"/>
     <col min="9" max="9" width="46.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="12" width="10.83203125" style="12"/>
@@ -826,17 +831,18 @@
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>36</v>
-      </c>
+      <c r="F2" s="9"/>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" s="8" t="s">
@@ -844,7 +850,7 @@
       </c>
       <c r="B3" s="9"/>
       <c r="C3" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" s="13">
         <v>1920</v>
@@ -852,6 +858,7 @@
       <c r="E3" s="13">
         <v>1080</v>
       </c>
+      <c r="F3" s="13"/>
       <c r="G3" s="13"/>
     </row>
     <row r="4" spans="1:14">
@@ -861,7 +868,6 @@
       <c r="B4" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="13"/>
       <c r="G4" s="13"/>
       <c r="H4" s="19"/>
     </row>
@@ -881,9 +887,7 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
-      <c r="E7" s="20" t="s">
-        <v>20</v>
-      </c>
+      <c r="E7" s="6"/>
       <c r="F7" s="20"/>
       <c r="G7" s="20"/>
       <c r="H7" s="6"/>
@@ -909,14 +913,14 @@
       <c r="D8" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>24</v>
+      <c r="E8" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="F8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>3</v>
@@ -948,20 +952,20 @@
         <v>19</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D9" s="2"/>
-      <c r="E9" s="11">
+      <c r="E9" s="2">
         <v>1</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I9" s="4" t="s">
         <v>17</v>
@@ -978,20 +982,20 @@
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="10">
+      <c r="E10" s="2">
         <v>2</v>
       </c>
       <c r="F10" s="10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G10" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="10"/>
@@ -1004,20 +1008,20 @@
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="10">
+      <c r="E11" s="2">
         <v>3</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G11" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="10"/>
@@ -1030,20 +1034,20 @@
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D12" s="2"/>
-      <c r="E12" s="10">
+      <c r="E12" s="2">
         <v>4</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="10"/>
@@ -1053,97 +1057,97 @@
       <c r="N12" s="2"/>
     </row>
     <row r="13" spans="1:14">
-      <c r="A13" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="B13" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="C13" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="F13" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="G13" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="H13" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="I13" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="J13" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="K13" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="L13" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="M13" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="N13" s="21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" ht="36">
-      <c r="A14" s="2">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2">
+        <v>5</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H13" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13" s="2"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="H14" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="I14" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="J14" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="K14" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="L14" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="M14" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="N14" s="21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" ht="36">
+      <c r="A15" s="2">
         <v>2</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="11">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2">
         <v>1</v>
       </c>
-      <c r="F14" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G14" s="11" t="s">
+      <c r="F15" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="H15" s="22" t="s">
         <v>52</v>
-      </c>
-      <c r="H14" s="22" t="s">
-        <v>53</v>
-      </c>
-      <c r="I14" s="2"/>
-      <c r="J14" s="10"/>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="10">
-        <v>2</v>
-      </c>
-      <c r="F15" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="G15" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="H15" s="17" t="s">
-        <v>40</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="10"/>
@@ -1152,26 +1156,26 @@
       <c r="M15" s="2"/>
       <c r="N15" s="2"/>
     </row>
-    <row r="16" spans="1:14" ht="18">
+    <row r="16" spans="1:14">
       <c r="A16" s="2"/>
-      <c r="B16" s="5"/>
+      <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D16" s="2"/>
-      <c r="E16" s="10">
-        <v>3</v>
+      <c r="E16" s="2">
+        <v>2</v>
       </c>
       <c r="F16" s="10" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G16" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="H16" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="I16" s="4"/>
+        <v>43</v>
+      </c>
+      <c r="H16" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="I16" s="2"/>
       <c r="J16" s="10"/>
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
@@ -1182,81 +1186,73 @@
       <c r="A17" s="2"/>
       <c r="B17" s="5"/>
       <c r="C17" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D17" s="2"/>
-      <c r="E17" s="10">
-        <v>4</v>
+      <c r="E17" s="2">
+        <v>3</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="G17" s="10" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="H17" s="16" t="s">
-        <v>40</v>
-      </c>
-      <c r="I17" s="2"/>
+        <v>55</v>
+      </c>
+      <c r="I17" s="4"/>
       <c r="J17" s="10"/>
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
       <c r="M17" s="2"/>
       <c r="N17" s="2"/>
     </row>
-    <row r="18" spans="1:14">
-      <c r="A18" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="B18" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="C18" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="F18" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="G18" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="H18" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="I18" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="J18" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="K18" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="L18" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="M18" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="N18" s="21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14">
+    <row r="18" spans="1:14" ht="18">
+      <c r="A18" s="2"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2">
+        <v>4</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H18" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="I18" s="2"/>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" spans="1:14" ht="18">
       <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="D19" s="2"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="10"/>
-      <c r="H19" s="17"/>
+      <c r="E19" s="2">
+        <v>5</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H19" s="16" t="s">
+        <v>39</v>
+      </c>
       <c r="I19" s="2"/>
       <c r="J19" s="10"/>
       <c r="K19" s="10"/>
@@ -1265,30 +1261,72 @@
       <c r="N19" s="2"/>
     </row>
     <row r="20" spans="1:14">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="10"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="10"/>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="2"/>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
+      <c r="A20" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="H20" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="I20" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="J20" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="K20" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="L20" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="M20" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="N20" s="21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="36">
+      <c r="A21" s="2">
+        <v>3</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>47</v>
+      </c>
       <c r="D21" s="2"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="10"/>
-      <c r="H21" s="17"/>
+      <c r="E21" s="2">
+        <v>1</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="H21" s="22" t="s">
+        <v>52</v>
+      </c>
       <c r="I21" s="2"/>
       <c r="J21" s="10"/>
       <c r="K21" s="10"/>
@@ -1299,12 +1337,22 @@
     <row r="22" spans="1:14">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
+      <c r="C22" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="D22" s="2"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="17"/>
+      <c r="E22" s="2">
+        <v>2</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="H22" s="17" t="s">
+        <v>39</v>
+      </c>
       <c r="I22" s="2"/>
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
@@ -1312,31 +1360,51 @@
       <c r="M22" s="2"/>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" ht="18">
       <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="2" t="s">
+        <v>49</v>
+      </c>
       <c r="D23" s="2"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="10"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="2"/>
+      <c r="E23" s="2">
+        <v>3</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H23" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="I23" s="4"/>
       <c r="J23" s="10"/>
       <c r="K23" s="10"/>
       <c r="L23" s="10"/>
       <c r="M23" s="2"/>
       <c r="N23" s="2"/>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" ht="18">
       <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="D24" s="2"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="17"/>
+      <c r="E24" s="2">
+        <v>4</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H24" s="16" t="s">
+        <v>39</v>
+      </c>
       <c r="I24" s="2"/>
       <c r="J24" s="10"/>
       <c r="K24" s="10"/>
@@ -1344,15 +1412,25 @@
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" ht="18">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
+      <c r="C25" s="2" t="s">
+        <v>57</v>
+      </c>
       <c r="D25" s="2"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="17"/>
+      <c r="E25" s="2">
+        <v>5</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H25" s="16" t="s">
+        <v>39</v>
+      </c>
       <c r="I25" s="2"/>
       <c r="J25" s="10"/>
       <c r="K25" s="10"/>
@@ -1361,27 +1439,55 @@
       <c r="N25" s="2"/>
     </row>
     <row r="26" spans="1:14">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="10"/>
-      <c r="F26" s="10"/>
-      <c r="G26" s="10"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="10"/>
-      <c r="K26" s="10"/>
-      <c r="L26" s="10"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
+      <c r="A26" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F26" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="G26" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="H26" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="I26" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="J26" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="K26" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="L26" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="M26" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="N26" s="21" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="27" spans="1:14">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="10"/>
+      <c r="E27" s="2"/>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
       <c r="H27" s="17"/>
@@ -1397,7 +1503,7 @@
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="10"/>
+      <c r="E28" s="2"/>
       <c r="F28" s="10"/>
       <c r="G28" s="10"/>
       <c r="H28" s="17"/>
@@ -1413,7 +1519,7 @@
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
-      <c r="E29" s="10"/>
+      <c r="E29" s="2"/>
       <c r="F29" s="10"/>
       <c r="G29" s="10"/>
       <c r="H29" s="17"/>
@@ -1429,7 +1535,7 @@
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
-      <c r="E30" s="10"/>
+      <c r="E30" s="2"/>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
       <c r="H30" s="17"/>
@@ -1445,7 +1551,7 @@
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
-      <c r="E31" s="10"/>
+      <c r="E31" s="2"/>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
       <c r="H31" s="17"/>
@@ -1461,7 +1567,7 @@
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
-      <c r="E32" s="10"/>
+      <c r="E32" s="2"/>
       <c r="F32" s="10"/>
       <c r="G32" s="10"/>
       <c r="H32" s="17"/>
@@ -1477,7 +1583,7 @@
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
-      <c r="E33" s="10"/>
+      <c r="E33" s="2"/>
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
       <c r="H33" s="17"/>
@@ -1493,7 +1599,7 @@
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
-      <c r="E34" s="10"/>
+      <c r="E34" s="2"/>
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
       <c r="H34" s="17"/>
@@ -1509,7 +1615,7 @@
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
-      <c r="E35" s="10"/>
+      <c r="E35" s="2"/>
       <c r="F35" s="10"/>
       <c r="G35" s="10"/>
       <c r="H35" s="17"/>
@@ -1525,7 +1631,7 @@
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
-      <c r="E36" s="10"/>
+      <c r="E36" s="2"/>
       <c r="F36" s="10"/>
       <c r="G36" s="10"/>
       <c r="H36" s="17"/>
@@ -1541,7 +1647,7 @@
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
-      <c r="E37" s="10"/>
+      <c r="E37" s="2"/>
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
       <c r="H37" s="17"/>
@@ -1557,7 +1663,7 @@
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
-      <c r="E38" s="10"/>
+      <c r="E38" s="2"/>
       <c r="F38" s="10"/>
       <c r="G38" s="10"/>
       <c r="H38" s="17"/>
@@ -1573,7 +1679,7 @@
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
-      <c r="E39" s="10"/>
+      <c r="E39" s="2"/>
       <c r="F39" s="10"/>
       <c r="G39" s="10"/>
       <c r="H39" s="17"/>
@@ -1584,29 +1690,62 @@
       <c r="M39" s="2"/>
       <c r="N39" s="2"/>
     </row>
+    <row r="40" spans="1:14">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="10"/>
+      <c r="G40" s="10"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="2"/>
+      <c r="J40" s="10"/>
+      <c r="K40" s="10"/>
+      <c r="L40" s="10"/>
+      <c r="M40" s="2"/>
+      <c r="N40" s="2"/>
+    </row>
+    <row r="41" spans="1:14">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="10"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="17"/>
+      <c r="I41" s="2"/>
+      <c r="J41" s="10"/>
+      <c r="K41" s="10"/>
+      <c r="L41" s="10"/>
+      <c r="M41" s="2"/>
+      <c r="N41" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="J7:L7"/>
-    <mergeCell ref="E7:G7"/>
+    <mergeCell ref="F7:G7"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F7" xr:uid="{16A1716D-893F-7D4E-B1E4-CC3888E279C4}">
       <formula1>"Input,Click,Find,Get"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6 E2:E5 F1 F9:F12 F14:F17 F19:F1048576" xr:uid="{BA56CD2A-7724-D940-ABD4-27EE5F4234E0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F6 F1:F3 F27:F1048576 F9:F13 F21:F25 F15:F19 E2:E3" xr:uid="{BA56CD2A-7724-D940-ABD4-27EE5F4234E0}">
       <formula1>"Input,Click,Find,Get,Screenshot,Clear,Wait"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1 J9:J12 J14:J17 J19:J1048576" xr:uid="{022DD76C-6569-1148-88FE-313A1245EF8C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1 J27:J1048576 J9:J13 J21:J25 J15:J19" xr:uid="{022DD76C-6569-1148-88FE-313A1245EF8C}">
       <formula1>"OK,NG,PENDING"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="C3" r:id="rId1" xr:uid="{C1C70E9A-0FBB-214B-A5F9-FD27C8722645}"/>
-    <hyperlink ref="H14" r:id="rId2" xr:uid="{31EA3A0C-56A9-1E4D-AE7B-3400D9CB9AB0}"/>
+    <hyperlink ref="H15" r:id="rId2" xr:uid="{31EA3A0C-56A9-1E4D-AE7B-3400D9CB9AB0}"/>
+    <hyperlink ref="H21" r:id="rId3" xr:uid="{7E16F446-5704-EB4C-B25F-399AE42A7BAE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -1622,37 +1761,37 @@
   <sheetData>
     <row r="2" spans="2:2">
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="2:2">
       <c r="B3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="2:2">
       <c r="B4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="2:2">
       <c r="B5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="2:2">
       <c r="B6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="2:2">
       <c r="B7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="2:2">
       <c r="B8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>